<commit_message>
Update Task 1 in C language coding dojang
</commit_message>
<xml_diff>
--- a/ToDoList.xlsx
+++ b/ToDoList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>인프런 버전관리 시스템 Git</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -66,6 +66,10 @@
   </si>
   <si>
     <t>Unit5. 변수 만들기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.2 변수 여러 개를 한 번에 선언하기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -171,9 +175,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -182,6 +183,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,7 +470,7 @@
   <dimension ref="A2:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -488,94 +492,96 @@
     </row>
     <row r="3" spans="1:7" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
@@ -587,84 +593,84 @@
     </row>
     <row r="15" spans="1:7" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
@@ -676,87 +682,92 @@
     </row>
     <row r="27" spans="1:7" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A16:A17"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A20:A21"/>
@@ -764,11 +775,6 @@
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A16:A17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update ToDoList.xlsx add outline
</commit_message>
<xml_diff>
--- a/ToDoList.xlsx
+++ b/ToDoList.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\02_GitRepoTortoise\01_Doc\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\works\04_Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CF6BEE-4F6B-414F-9819-858C8B2B5E3C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,10 +35,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>GIT2-CLI 버전관리편</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Task2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -70,14 +67,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>삭제 - git reset</t>
+    <t>GIT3-CLI 백업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Push</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -467,11 +468,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -484,7 +485,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -497,10 +498,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -513,7 +514,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -522,31 +523,31 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
-      <c r="B7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -566,14 +567,14 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
@@ -615,7 +616,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -635,7 +636,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -655,7 +656,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -704,7 +705,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -724,7 +725,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -744,7 +745,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -764,6 +765,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A16:A17"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A20:A21"/>
@@ -771,11 +777,6 @@
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A16:A17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MAP add in ToDoList.xlsx
</commit_message>
<xml_diff>
--- a/ToDoList.xlsx
+++ b/ToDoList.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\works\04_Git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\02_GitRepoTortoise\01_Doc\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F67D41E-ADF0-429D-9E71-0913A16F0F44}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ToDo" sheetId="1" r:id="rId1"/>
+    <sheet name="MAP" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="65">
   <si>
     <t>인프런 버전관리 시스템 Git</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -80,14 +80,218 @@
   </si>
   <si>
     <t>인프런 지옥에서 온 Git</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Massive Action Plan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Why</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>By When</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description of Massive Action to be taken</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Action steps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Potentional Barriers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Positive affirmation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영어 훈련 1단계를 완성한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>원어민들과 자유롭고 행복하게 영어로 대화하고 싶다. 직장에서도 영어가 나의 무기가 된다. 영어로 멋있게 프레젠테이션 할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018년 9월 30일까지 완성한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 기상시간 5시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알람을 꺼버릴 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알람을 3개 켜자.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일어나서 바로 샤워하자.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 음소단위 하루 3개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   훈련</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>귀찮아서 안할 수 있으니 씻기 전에 거울 보면서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연습한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 하루 영화 20문장 소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   리 분석 훈련</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>각 문장마다 편해질 때까지 반복 연습, 적어도 한 문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장 10번 이상.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. 한글 보고 영어로 말</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>훈련한 소리 그대로 반복해서 영어로 말한다. 5번 이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상 반복한다. 암기하려고 애쓰지 않는다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. MP3 파일 따라 듣고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   다니기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하루 종일 연습한 소리를 듣고 따라한다. 통근 길에,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>점심 먹고 30분 동안, 적어도 1시간 짬을 낸다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N 바빠서 시간이 없었다. 다음에는 먼저 해야지.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. 전에 훈련한 문장 체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   화 복습</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한글을 보고 영어로 말한다. 헷갈리는 문장은 다시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소리 연습한다. 3번.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. I am great and wonderful.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. I am the architect of my life.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. I am superior to negative thoughts and low actions.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Example]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,16 +307,50 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -172,13 +410,94 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -196,6 +515,99 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -476,10 +888,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -777,6 +1189,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A16:A17"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A20:A21"/>
@@ -784,14 +1201,426 @@
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A16:A17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.75" customWidth="1"/>
+    <col min="2" max="2" width="44.25" customWidth="1"/>
+    <col min="3" max="3" width="18.25" customWidth="1"/>
+    <col min="5" max="5" width="19.75" customWidth="1"/>
+    <col min="6" max="6" width="44.25" customWidth="1"/>
+    <col min="7" max="7" width="18.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="E2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="19"/>
+      <c r="G2" s="20"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="E3" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="16">
+        <v>43282</v>
+      </c>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="E4" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="E5" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="E6" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="E7" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="23"/>
+      <c r="G7" s="24"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="E9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="32"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="33"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="E12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="8"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="E13" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="32"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="33"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="2"/>
+      <c r="E15" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="3"/>
+      <c r="E16" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="32"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="4"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="33"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="E18" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="8"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="E19" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="32"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="33"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="E21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="8"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="E22" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="35"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="36"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="E24" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="E25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" s="32"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="33"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="E27" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="29"/>
+      <c r="B28" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="15"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28" s="15"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="30"/>
+      <c r="B29" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="26">
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A7:C7"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A9 A12 A15 A18 A21 A24 B27:B29" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update and add new file
</commit_message>
<xml_diff>
--- a/ToDoList.xlsx
+++ b/ToDoList.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="105">
   <si>
     <t>Task1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -288,10 +288,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Virtual Box 환경설정 ST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>.so library ST</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -425,6 +421,30 @@
   </si>
   <si>
     <t>5.4 퀴즈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Virtual Box 설치,환경설정 ST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Virtual Box Ubuntu 설치, 환경설정ST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SS BBUe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Init 구조 ST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GOM FPGA, Device Driver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Installation UI</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -702,6 +722,36 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -719,36 +769,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1033,7 +1053,7 @@
   <dimension ref="A2:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1068,7 +1088,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1077,13 +1097,13 @@
       <c r="A5" s="11"/>
       <c r="B5" s="4"/>
       <c r="C5" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -1152,7 +1172,9 @@
       <c r="B14" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1164,9 +1186,11 @@
         <v>0</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1177,7 +1201,9 @@
       <c r="B17" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -1188,9 +1214,11 @@
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -1209,7 +1237,9 @@
       <c r="A20" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -1336,6 +1366,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A16:A17"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A20:A21"/>
@@ -1343,11 +1378,6 @@
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A16:A17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1379,84 +1409,84 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
-      <c r="E2" s="27" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="E2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="29"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
       <c r="E3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="24">
         <v>43282</v>
       </c>
-      <c r="G3" s="31"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
       <c r="E4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="31"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
       <c r="E5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="32"/>
+      <c r="G5" s="26"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
       <c r="E6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="31"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="35"/>
-      <c r="E7" s="33" t="s">
+      <c r="B7" s="28"/>
+      <c r="C7" s="29"/>
+      <c r="E7" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="34"/>
-      <c r="G7" s="35"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
@@ -1490,7 +1520,7 @@
       <c r="F9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="31" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1504,7 +1534,7 @@
       <c r="F10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="22"/>
+      <c r="G10" s="32"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
@@ -1514,7 +1544,7 @@
       <c r="F11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="23"/>
+      <c r="G11" s="33"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
@@ -1528,7 +1558,7 @@
       <c r="F12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="G12" s="31" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1542,7 +1572,7 @@
       <c r="F13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="22"/>
+      <c r="G13" s="32"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
@@ -1550,7 +1580,7 @@
       <c r="C14" s="4"/>
       <c r="E14" s="6"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="23"/>
+      <c r="G14" s="33"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
@@ -1564,7 +1594,7 @@
       <c r="F15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="31" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1578,7 +1608,7 @@
       <c r="F16" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="22"/>
+      <c r="G16" s="32"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
@@ -1586,7 +1616,7 @@
       <c r="C17" s="4"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="23"/>
+      <c r="G17" s="33"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
@@ -1600,7 +1630,7 @@
       <c r="F18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G18" s="21" t="s">
+      <c r="G18" s="31" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1614,7 +1644,7 @@
       <c r="F19" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G19" s="22"/>
+      <c r="G19" s="32"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
@@ -1622,7 +1652,7 @@
       <c r="C20" s="4"/>
       <c r="E20" s="6"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="23"/>
+      <c r="G20" s="33"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
@@ -1636,7 +1666,7 @@
       <c r="F21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G21" s="24" t="s">
+      <c r="G21" s="34" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1650,7 +1680,7 @@
       <c r="F22" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G22" s="25"/>
+      <c r="G22" s="35"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
@@ -1658,7 +1688,7 @@
       <c r="C23" s="4"/>
       <c r="E23" s="6"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="26"/>
+      <c r="G23" s="36"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
@@ -1672,7 +1702,7 @@
       <c r="F24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G24" s="21" t="s">
+      <c r="G24" s="31" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1686,7 +1716,7 @@
       <c r="F25" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G25" s="22"/>
+      <c r="G25" s="32"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
@@ -1694,7 +1724,7 @@
       <c r="C26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="23"/>
+      <c r="G26" s="33"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
@@ -1738,6 +1768,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="G24:G26"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
@@ -1754,16 +1794,6 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="A7:C7"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="G24:G26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1790,7 +1820,7 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
@@ -1798,7 +1828,7 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
@@ -1806,13 +1836,13 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" t="s">
         <v>77</v>
-      </c>
-      <c r="D6" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
@@ -1823,7 +1853,7 @@
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
@@ -1831,7 +1861,7 @@
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
@@ -1839,7 +1869,7 @@
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
@@ -1847,13 +1877,13 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
@@ -1864,7 +1894,7 @@
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
@@ -1872,92 +1902,92 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update BookRecorder.xlsx and ToDoList.xlsx
</commit_message>
<xml_diff>
--- a/ToDoList.xlsx
+++ b/ToDoList.xlsx
@@ -453,14 +453,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Virtual Box 환경설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Eth, Qt5 Install</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Serial Port setup and test</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -518,6 +510,14 @@
   </si>
   <si>
     <t>선정된 커뮤니티에 질문하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Virtual Box</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S006_Tips~.docx(Eth, Qt5 Install)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -795,6 +795,36 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -812,36 +842,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1126,7 +1126,7 @@
   <dimension ref="A2:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1139,7 +1139,7 @@
         <v>98</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
@@ -1148,7 +1148,7 @@
         <v>97</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -1167,10 +1167,10 @@
         <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G4" s="2"/>
     </row>
@@ -1186,10 +1186,10 @@
         <v>7</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G5" s="3"/>
     </row>
@@ -1202,7 +1202,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -1224,7 +1224,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G8" s="3"/>
     </row>
@@ -1275,7 +1275,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>100</v>
@@ -1288,7 +1288,7 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="4" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>95</v>
@@ -1316,7 +1316,7 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
       <c r="B19" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>101</v>
@@ -1344,7 +1344,7 @@
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
       <c r="B21" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>103</v>
@@ -1467,6 +1467,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A16:A17"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A20:A21"/>
@@ -1474,11 +1479,6 @@
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A16:A17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1510,84 +1510,84 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
-      <c r="E2" s="27" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="E2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="29"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
       <c r="E3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="24">
         <v>43282</v>
       </c>
-      <c r="G3" s="31"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
       <c r="E4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="31"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
       <c r="E5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="32"/>
+      <c r="G5" s="26"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
       <c r="E6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="31"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="35"/>
-      <c r="E7" s="33" t="s">
+      <c r="B7" s="28"/>
+      <c r="C7" s="29"/>
+      <c r="E7" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="34"/>
-      <c r="G7" s="35"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
@@ -1621,7 +1621,7 @@
       <c r="F9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="31" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1635,7 +1635,7 @@
       <c r="F10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="22"/>
+      <c r="G10" s="32"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
@@ -1645,7 +1645,7 @@
       <c r="F11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="23"/>
+      <c r="G11" s="33"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
@@ -1659,7 +1659,7 @@
       <c r="F12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="G12" s="31" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1673,7 +1673,7 @@
       <c r="F13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="22"/>
+      <c r="G13" s="32"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
@@ -1681,7 +1681,7 @@
       <c r="C14" s="4"/>
       <c r="E14" s="6"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="23"/>
+      <c r="G14" s="33"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
@@ -1695,7 +1695,7 @@
       <c r="F15" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="31" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1709,7 +1709,7 @@
       <c r="F16" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="22"/>
+      <c r="G16" s="32"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
@@ -1717,7 +1717,7 @@
       <c r="C17" s="4"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="23"/>
+      <c r="G17" s="33"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
@@ -1731,7 +1731,7 @@
       <c r="F18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G18" s="21" t="s">
+      <c r="G18" s="31" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1745,7 +1745,7 @@
       <c r="F19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="22"/>
+      <c r="G19" s="32"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
@@ -1753,7 +1753,7 @@
       <c r="C20" s="4"/>
       <c r="E20" s="6"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="23"/>
+      <c r="G20" s="33"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
@@ -1767,7 +1767,7 @@
       <c r="F21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G21" s="24" t="s">
+      <c r="G21" s="34" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1781,7 +1781,7 @@
       <c r="F22" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G22" s="25"/>
+      <c r="G22" s="35"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
@@ -1789,7 +1789,7 @@
       <c r="C23" s="4"/>
       <c r="E23" s="6"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="26"/>
+      <c r="G23" s="36"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
@@ -1803,7 +1803,7 @@
       <c r="F24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G24" s="21" t="s">
+      <c r="G24" s="31" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1817,7 +1817,7 @@
       <c r="F25" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G25" s="22"/>
+      <c r="G25" s="32"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
@@ -1825,7 +1825,7 @@
       <c r="C26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="23"/>
+      <c r="G26" s="33"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
@@ -1869,6 +1869,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="G24:G26"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
@@ -1885,16 +1895,6 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="A7:C7"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="G24:G26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2109,27 +2109,27 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>